<commit_message>
wg test correction #2
Former-commit-id: 586070e448b43da3fb27169a71b9f27c426a9ec3
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_wg.xlsx
+++ b/tests/test_data/test_dfs_wg.xlsx
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,11 +1378,11 @@
       </c>
       <c r="AB5" s="13">
         <f>1.08*(AO5-((AI5+(AJ5*AO5)+(AK5*AN5))*AN5))</f>
-        <v>280.32774057000006</v>
+        <v>244.81431657000002</v>
       </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AE5" s="11">
         <f t="shared" si="2"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="AH5" s="12">
         <f t="shared" si="3"/>
-        <v>585</v>
+        <v>665</v>
       </c>
       <c r="AI5" s="9">
         <v>5.7000000000000002E-2</v>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="AN5" s="12">
         <f t="shared" si="4"/>
-        <v>585</v>
+        <v>665</v>
       </c>
       <c r="AO5">
         <f t="shared" si="5"/>
@@ -1508,10 +1508,10 @@
       </c>
       <c r="AB6" s="13">
         <f>1.08*(AO6-((AI6+(AJ6*AO6)+(AK6*AN6))*AN6))</f>
-        <v>280.32774057000006</v>
+        <v>244.81431657000002</v>
       </c>
       <c r="AD6" s="3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AE6" s="10">
         <f t="shared" si="2"/>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="AH6" s="12">
         <f t="shared" si="3"/>
-        <v>585</v>
+        <v>665</v>
       </c>
       <c r="AI6" s="6">
         <v>5.7000000000000002E-2</v>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="AN6" s="12">
         <f t="shared" si="4"/>
-        <v>585</v>
+        <v>665</v>
       </c>
       <c r="AO6">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
heating costs do not matter for housing benefit!
Former-commit-id: cfbd7e22362c6a026cc3a24d5f1fb4358ca87253
Former-commit-id: 8e882c179b3615c10a4fb7233195c9451a73076b
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_wg.xlsx
+++ b/tests/test_data/test_dfs_wg.xlsx
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="AC2" s="13">
         <f>1.15*(AP2-((AJ2+(AK2*AP2)+(AL2*AO2))*AO2))</f>
-        <v>112.28878874999987</v>
+        <v>60.43528875000009</v>
       </c>
       <c r="AE2">
         <v>0.3</v>
@@ -1040,8 +1040,8 @@
         <v>1445</v>
       </c>
       <c r="AP2">
-        <f>ROUND(MAX(MIN(H2,AM2)+I2,AN2)+4,-1)-5</f>
-        <v>665</v>
+        <f>ROUND(MAX(MIN(H2,AM2),AN2)+4,-1)-5</f>
+        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="AC3" s="13">
         <f t="shared" ref="AC3:AC4" si="1">1.15*(AP3-((AJ3+(AK3*AP3)+(AL3*AO3))*AO3))</f>
-        <v>112.28878874999987</v>
+        <v>60.43528875000009</v>
       </c>
       <c r="AE3">
         <v>0.3</v>
@@ -1172,8 +1172,8 @@
         <v>1445</v>
       </c>
       <c r="AP3">
-        <f t="shared" ref="AP3:AP13" si="5">ROUND(MAX(MIN(H3,AM3)+I3,AN3)+4,-1)-5</f>
-        <v>665</v>
+        <f t="shared" ref="AP3:AP13" si="5">ROUND(MAX(MIN(H3,AM3),AN3)+4,-1)-5</f>
+        <v>565</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="AC4" s="13">
         <f t="shared" si="1"/>
-        <v>112.28878874999987</v>
+        <v>60.43528875000009</v>
       </c>
       <c r="AE4">
         <v>0.3</v>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="AP4">
         <f t="shared" si="5"/>
-        <v>665</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AC5" s="13">
         <f>1.08*(AP5-((AJ5+(AK5*AP5)+(AL5*AO5))*AO5))</f>
-        <v>244.81431657000002</v>
+        <v>191.51471817000001</v>
       </c>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="AP5">
         <f t="shared" si="5"/>
-        <v>475</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="AC6" s="13">
         <f>1.08*(AP6-((AJ6+(AK6*AP6)+(AL6*AO6))*AO6))</f>
-        <v>244.81431657000002</v>
+        <v>191.51471817000001</v>
       </c>
       <c r="AE6" s="3">
         <v>0.2</v>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="AP6">
         <f t="shared" si="5"/>
-        <v>475</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
@@ -1633,8 +1633,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <f>1400*12</f>
-        <v>16800</v>
+        <v>16000</v>
       </c>
       <c r="U7" s="2">
         <v>0</v>
@@ -1662,7 +1661,7 @@
       </c>
       <c r="AC7" s="13">
         <f t="shared" ref="AC7:AC8" si="6">1.08*(AP7-((AJ7+(AK7*AP7)+(AL7*AO7))*AO7))</f>
-        <v>28.486336770000033</v>
+        <v>15.962717249999999</v>
       </c>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2">
@@ -1670,18 +1669,18 @@
       </c>
       <c r="AF7" s="11">
         <f t="shared" si="2"/>
-        <v>1650</v>
+        <v>1583.3333333333333</v>
       </c>
       <c r="AG7" s="10">
         <f>SUM($AF$7:$AF$8)</f>
-        <v>1650</v>
+        <v>1583.3333333333333</v>
       </c>
       <c r="AH7" s="2">
         <v>50</v>
       </c>
       <c r="AI7" s="12">
         <f t="shared" si="3"/>
-        <v>1115</v>
+        <v>1075</v>
       </c>
       <c r="AJ7" s="9">
         <v>5.7000000000000002E-2</v>
@@ -1700,11 +1699,11 @@
       </c>
       <c r="AO7" s="12">
         <f t="shared" si="4"/>
-        <v>1115</v>
+        <v>1075</v>
       </c>
       <c r="AP7">
         <f t="shared" si="5"/>
-        <v>475</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
@@ -1795,7 +1794,7 @@
       </c>
       <c r="AC8" s="13">
         <f t="shared" si="6"/>
-        <v>28.486336770000033</v>
+        <v>15.962717249999999</v>
       </c>
       <c r="AE8" s="3">
         <v>0.3</v>
@@ -1806,14 +1805,14 @@
       </c>
       <c r="AG8" s="10">
         <f>SUM($AF$7:$AF$8)</f>
-        <v>1650</v>
+        <v>1583.3333333333333</v>
       </c>
       <c r="AH8" s="3">
         <v>50</v>
       </c>
       <c r="AI8" s="12">
         <f t="shared" si="3"/>
-        <v>1115</v>
+        <v>1075</v>
       </c>
       <c r="AJ8" s="6">
         <v>5.7000000000000002E-2</v>
@@ -1832,11 +1831,11 @@
       </c>
       <c r="AO8" s="12">
         <f t="shared" si="4"/>
-        <v>1115</v>
+        <v>1075</v>
       </c>
       <c r="AP8">
         <f t="shared" si="5"/>
-        <v>475</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
@@ -1927,7 +1926,7 @@
       </c>
       <c r="AC9" s="13">
         <f>(AP9-((AJ9+(AK9*AP9)+(AL9*AO9))*AO9))</f>
-        <v>612.35275024999999</v>
+        <v>504.25435025000002</v>
       </c>
       <c r="AD9" s="2"/>
       <c r="AE9" s="2">
@@ -1968,7 +1967,7 @@
       </c>
       <c r="AP9">
         <f t="shared" si="5"/>
-        <v>695</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
@@ -2059,7 +2058,7 @@
       </c>
       <c r="AC10" s="13">
         <f t="shared" ref="AC10:AC13" si="7">(AP10-((AJ10+(AK10*AP10)+(AL10*AO10))*AO10))</f>
-        <v>612.35275024999999</v>
+        <v>504.25435025000002</v>
       </c>
       <c r="AE10" s="3">
         <v>0.1</v>
@@ -2099,7 +2098,7 @@
       </c>
       <c r="AP10">
         <f t="shared" si="5"/>
-        <v>695</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -2190,7 +2189,7 @@
       </c>
       <c r="AC11" s="13">
         <f t="shared" si="7"/>
-        <v>612.35275024999999</v>
+        <v>504.25435025000002</v>
       </c>
       <c r="AE11" s="3">
         <v>0.1</v>
@@ -2230,7 +2229,7 @@
       </c>
       <c r="AP11">
         <f t="shared" si="5"/>
-        <v>695</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
@@ -2321,7 +2320,7 @@
       </c>
       <c r="AC12" s="13">
         <f t="shared" si="7"/>
-        <v>612.35275024999999</v>
+        <v>504.25435025000002</v>
       </c>
       <c r="AE12" s="3">
         <v>0.1</v>
@@ -2361,7 +2360,7 @@
       </c>
       <c r="AP12">
         <f t="shared" si="5"/>
-        <v>695</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
@@ -2452,7 +2451,7 @@
       </c>
       <c r="AC13" s="13">
         <f t="shared" si="7"/>
-        <v>612.35275024999999</v>
+        <v>504.25435025000002</v>
       </c>
       <c r="AE13" s="3">
         <v>0.1</v>
@@ -2492,7 +2491,7 @@
       </c>
       <c r="AP13">
         <f t="shared" si="5"/>
-        <v>695</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>